<commit_message>
merged level 3 'Other neglected tropical diseases'
</commit_message>
<xml_diff>
--- a/data-raw/mastercauselist.xlsx
+++ b/data-raw/mastercauselist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="636">
   <si>
     <t>Level1</t>
   </si>
@@ -1859,9 +1859,6 @@
   </si>
   <si>
     <t>Cutaneous and mucocutaneous leishmaniasis</t>
-  </si>
-  <si>
-    <t>Leishmaniasis</t>
   </si>
   <si>
     <t>std_gonnorhea</t>
@@ -2322,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,7 +2480,7 @@
         <v>274</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>569</v>
@@ -2492,7 +2489,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2552,7 +2549,7 @@
         <v>274</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>572</v>
@@ -2561,7 +2558,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,16 +2687,16 @@
         <v>274</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F16" s="2">
         <v>14</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2716,7 +2713,7 @@
         <v>122</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F17" s="2">
         <v>15</v>
@@ -2739,7 +2736,7 @@
         <v>544</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F18" s="2">
         <v>16</v>
@@ -3193,7 +3190,7 @@
         <v>225</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>594</v>
+        <v>135</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>594</v>
@@ -3216,7 +3213,7 @@
         <v>225</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>48</v>
+        <v>135</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>48</v>
@@ -3239,7 +3236,7 @@
         <v>225</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>248</v>
+        <v>135</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>248</v>
@@ -3262,7 +3259,7 @@
         <v>225</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>606</v>
+        <v>135</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>606</v>
@@ -3285,7 +3282,7 @@
         <v>225</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>609</v>
+        <v>135</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>609</v>
@@ -3308,7 +3305,7 @@
         <v>225</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>540</v>
+        <v>135</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>540</v>
@@ -3331,7 +3328,7 @@
         <v>225</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>543</v>
+        <v>135</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>543</v>
@@ -3354,7 +3351,7 @@
         <v>225</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>615</v>
+        <v>135</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>614</v>
@@ -3377,10 +3374,10 @@
         <v>225</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>631</v>
+        <v>135</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>612</v>
@@ -3389,7 +3386,7 @@
         <v>44</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3406,7 +3403,7 @@
         <v>135</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F47" s="3">
         <v>45</v>
@@ -3610,7 +3607,7 @@
         <v>556</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>566</v>
@@ -3619,7 +3616,7 @@
         <v>54</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3636,7 +3633,7 @@
         <v>542</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F57" s="3">
         <v>55</v>
@@ -4136,14 +4133,14 @@
         <v>175</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2">
         <v>78</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4199,14 +4196,14 @@
         <v>175</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2">
         <v>81</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -5354,14 +5351,14 @@
         <v>120</v>
       </c>
       <c r="D138" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E138" s="2"/>
       <c r="F138" s="2">
         <v>136</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update master cause list & ICD-GDB-mapping
</commit_message>
<xml_diff>
--- a/data-raw/mastercauselist.xlsx
+++ b/data-raw/mastercauselist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514004A4-F7C8-44CD-AE2D-5C0305C9ECD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFAD0ED-6995-487A-B2DB-1353850DC752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="683">
   <si>
     <t>Level1</t>
   </si>
@@ -1993,9 +1993,6 @@
     <t>Soft tissues cancer</t>
   </si>
   <si>
-    <t>Other female organs cancer</t>
-  </si>
-  <si>
     <t>Vulva cancer</t>
   </si>
   <si>
@@ -2035,15 +2032,9 @@
     <t>Thymus cancer</t>
   </si>
   <si>
-    <t>Heart, mediastinum and pleura cancer</t>
-  </si>
-  <si>
     <t>Bone and articular cartilage cancers, nos</t>
   </si>
   <si>
-    <t>Bone and articular cartilage of limbs cancers</t>
-  </si>
-  <si>
     <t>neo_bone_cancer_nos</t>
   </si>
   <si>
@@ -2069,6 +2060,15 @@
   </si>
   <si>
     <t>neo_female_cancer_placenta</t>
+  </si>
+  <si>
+    <t>Other female genital organs</t>
+  </si>
+  <si>
+    <t>neo_otherfemale_cancer</t>
+  </si>
+  <si>
+    <t>Heart, mediastinum and pleura cancers</t>
   </si>
 </sst>
 </file>
@@ -2172,10 +2172,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G278" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A1:G278" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G259">
-    <sortCondition ref="E1:E259"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G279" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A1:G279" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G260">
+    <sortCondition ref="E1:E260"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Level1" dataCellStyle="Normal"/>
@@ -2511,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G278"/>
+  <dimension ref="A1:G279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C209" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D244" sqref="D244"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I212" sqref="I212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6953,7 +6953,7 @@
         <v>654</v>
       </c>
       <c r="D205" s="5" t="s">
-        <v>673</v>
+        <v>654</v>
       </c>
       <c r="G205" s="5" t="s">
         <v>655</v>
@@ -6970,10 +6970,10 @@
         <v>654</v>
       </c>
       <c r="D206" s="5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G206" s="5" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -7131,13 +7131,13 @@
         <v>199</v>
       </c>
       <c r="C214" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="D214" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="G214" s="5" t="s">
         <v>665</v>
-      </c>
-      <c r="D214" s="5" t="s">
-        <v>665</v>
-      </c>
-      <c r="G214" s="5" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -7505,13 +7505,13 @@
         <v>199</v>
       </c>
       <c r="C232" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="D232" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="D232" s="5" t="s">
-        <v>658</v>
-      </c>
       <c r="G232" s="5" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="233" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7522,13 +7522,13 @@
         <v>199</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>657</v>
+        <v>680</v>
       </c>
       <c r="D233" s="5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G233" s="5" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="234" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7539,34 +7539,30 @@
         <v>199</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>657</v>
+        <v>680</v>
       </c>
       <c r="D234" s="5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G234" s="5" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
-        <v>200</v>
-      </c>
-      <c r="B235" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B235" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C235" t="s">
-        <v>131</v>
-      </c>
-      <c r="D235" t="s">
-        <v>131</v>
-      </c>
-      <c r="E235" s="2"/>
-      <c r="F235">
-        <v>225</v>
-      </c>
-      <c r="G235" t="s">
-        <v>340</v>
+      <c r="C235" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="G235" s="5" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -7577,17 +7573,17 @@
         <v>199</v>
       </c>
       <c r="C236" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D236" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E236" s="2"/>
       <c r="F236">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G236" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -7598,17 +7594,17 @@
         <v>199</v>
       </c>
       <c r="C237" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D237" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E237" s="2"/>
       <c r="F237">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G237" t="s">
-        <v>353</v>
+        <v>368</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -7619,72 +7615,76 @@
         <v>199</v>
       </c>
       <c r="C238" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D238" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E238" s="2"/>
       <c r="F238">
+        <v>227</v>
+      </c>
+      <c r="G238" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>200</v>
+      </c>
+      <c r="B239" t="s">
+        <v>199</v>
+      </c>
+      <c r="C239" t="s">
+        <v>147</v>
+      </c>
+      <c r="D239" t="s">
+        <v>147</v>
+      </c>
+      <c r="E239" s="2"/>
+      <c r="F239">
         <v>228</v>
       </c>
-      <c r="G238" t="s">
+      <c r="G239" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="239" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B239" s="5" t="s">
+    <row r="240" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B240" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C239" s="5" t="s">
+      <c r="C240" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="G240" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="D239" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="G239" s="5" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
-        <v>200</v>
-      </c>
-      <c r="B240" t="s">
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>200</v>
+      </c>
+      <c r="B241" t="s">
         <v>199</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C241" t="s">
         <v>161</v>
       </c>
-      <c r="D240" t="s">
+      <c r="D241" t="s">
         <v>161</v>
       </c>
-      <c r="E240" s="2"/>
-      <c r="F240">
+      <c r="E241" s="2"/>
+      <c r="F241">
         <v>229</v>
       </c>
-      <c r="G240" t="s">
+      <c r="G241" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C241" s="5" t="s">
-        <v>651</v>
-      </c>
-      <c r="D241" s="5" t="s">
-        <v>651</v>
-      </c>
-      <c r="G241" s="5" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="242" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7695,13 +7695,13 @@
         <v>199</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D242" s="5" t="s">
-        <v>667</v>
+        <v>651</v>
       </c>
       <c r="G242" s="5" t="s">
-        <v>677</v>
+        <v>652</v>
       </c>
     </row>
     <row r="243" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7715,10 +7715,10 @@
         <v>656</v>
       </c>
       <c r="D243" s="5" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G243" s="5" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="244" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7732,31 +7732,27 @@
         <v>656</v>
       </c>
       <c r="D244" s="5" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G244" s="5" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
-        <v>200</v>
-      </c>
-      <c r="B245" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B245" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C245" t="s">
-        <v>179</v>
-      </c>
-      <c r="D245" t="s">
-        <v>263</v>
-      </c>
-      <c r="E245" s="2"/>
-      <c r="F245">
-        <v>230</v>
-      </c>
-      <c r="G245" t="s">
-        <v>443</v>
+      <c r="C245" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="D245" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="G245" s="5" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -7770,14 +7766,14 @@
         <v>179</v>
       </c>
       <c r="D246" t="s">
-        <v>179</v>
+        <v>263</v>
       </c>
       <c r="E246" s="2"/>
       <c r="F246">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G246" t="s">
-        <v>339</v>
+        <v>443</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -7788,17 +7784,17 @@
         <v>199</v>
       </c>
       <c r="C247" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D247" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E247" s="2"/>
       <c r="F247">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G247" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -7809,34 +7805,38 @@
         <v>199</v>
       </c>
       <c r="C248" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D248" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E248" s="2"/>
       <c r="F248">
+        <v>232</v>
+      </c>
+      <c r="G248" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>200</v>
+      </c>
+      <c r="B249" t="s">
+        <v>199</v>
+      </c>
+      <c r="C249" t="s">
+        <v>185</v>
+      </c>
+      <c r="D249" t="s">
+        <v>185</v>
+      </c>
+      <c r="E249" s="2"/>
+      <c r="F249">
         <v>233</v>
       </c>
-      <c r="G248" t="s">
+      <c r="G249" t="s">
         <v>359</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B249" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C249" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="D249" s="5" t="s">
-        <v>670</v>
-      </c>
-      <c r="G249" s="5" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="250" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -7850,69 +7850,65 @@
         <v>653</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G250" s="5" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
-        <v>200</v>
-      </c>
-      <c r="B251" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A251" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B251" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="D251" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="G251" s="5" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>200</v>
+      </c>
+      <c r="B252" t="s">
+        <v>199</v>
+      </c>
+      <c r="C252" t="s">
         <v>186</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D252" t="s">
         <v>186</v>
       </c>
-      <c r="E251" s="2"/>
-      <c r="F251">
+      <c r="E252" s="2"/>
+      <c r="F252">
         <v>234</v>
       </c>
-      <c r="G251" t="s">
+      <c r="G252" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="252" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A252" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B252" s="5" t="s">
+    <row r="253" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A253" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B253" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C252" s="5" t="s">
+      <c r="C253" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="G253" s="5" t="s">
         <v>661</v>
-      </c>
-      <c r="D252" s="5" t="s">
-        <v>661</v>
-      </c>
-      <c r="G252" s="5" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A253" t="s">
-        <v>200</v>
-      </c>
-      <c r="B253" t="s">
-        <v>199</v>
-      </c>
-      <c r="C253" t="s">
-        <v>193</v>
-      </c>
-      <c r="D253" t="s">
-        <v>193</v>
-      </c>
-      <c r="E253" s="2"/>
-      <c r="F253">
-        <v>235</v>
-      </c>
-      <c r="G253" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -7920,20 +7916,20 @@
         <v>200</v>
       </c>
       <c r="B254" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C254" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="D254" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="E254" s="2"/>
       <c r="F254">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G254" t="s">
-        <v>388</v>
+        <v>352</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -7944,17 +7940,17 @@
         <v>201</v>
       </c>
       <c r="C255" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="D255" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="E255" s="2"/>
       <c r="F255">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G255" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -7965,17 +7961,17 @@
         <v>201</v>
       </c>
       <c r="C256" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="D256" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="E256" s="2"/>
       <c r="F256">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G256" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -7986,17 +7982,17 @@
         <v>201</v>
       </c>
       <c r="C257" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D257" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E257" s="2"/>
       <c r="F257">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G257" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -8007,17 +8003,17 @@
         <v>201</v>
       </c>
       <c r="C258" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="D258" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="E258" s="2"/>
       <c r="F258">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G258" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -8031,14 +8027,14 @@
         <v>137</v>
       </c>
       <c r="D259" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E259" s="2"/>
       <c r="F259">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G259" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -8052,14 +8048,14 @@
         <v>137</v>
       </c>
       <c r="D260" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="E260" s="2"/>
       <c r="F260">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G260" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -8070,17 +8066,17 @@
         <v>201</v>
       </c>
       <c r="C261" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D261" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E261" s="2"/>
       <c r="F261">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G261" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -8088,20 +8084,20 @@
         <v>200</v>
       </c>
       <c r="B262" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C262" t="s">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="D262" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="E262" s="2"/>
       <c r="F262">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G262" t="s">
-        <v>489</v>
+        <v>400</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -8111,18 +8107,18 @@
       <c r="B263" t="s">
         <v>205</v>
       </c>
-      <c r="C263" s="2" t="s">
+      <c r="C263" t="s">
         <v>224</v>
       </c>
-      <c r="D263" s="2" t="s">
-        <v>525</v>
+      <c r="D263" t="s">
+        <v>32</v>
       </c>
       <c r="E263" s="2"/>
-      <c r="F263" s="2">
-        <v>245</v>
-      </c>
-      <c r="G263" s="2" t="s">
-        <v>530</v>
+      <c r="F263">
+        <v>244</v>
+      </c>
+      <c r="G263" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -8132,18 +8128,18 @@
       <c r="B264" t="s">
         <v>205</v>
       </c>
-      <c r="C264" t="s">
+      <c r="C264" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D264" t="s">
-        <v>44</v>
+      <c r="D264" s="2" t="s">
+        <v>525</v>
       </c>
       <c r="E264" s="2"/>
-      <c r="F264">
-        <v>246</v>
-      </c>
-      <c r="G264" t="s">
-        <v>486</v>
+      <c r="F264" s="2">
+        <v>245</v>
+      </c>
+      <c r="G264" s="2" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -8157,14 +8153,14 @@
         <v>224</v>
       </c>
       <c r="D265" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E265" s="2"/>
       <c r="F265">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G265" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
@@ -8178,14 +8174,14 @@
         <v>224</v>
       </c>
       <c r="D266" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E266" s="2"/>
       <c r="F266">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G266" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
@@ -8199,14 +8195,14 @@
         <v>224</v>
       </c>
       <c r="D267" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E267" s="2"/>
       <c r="F267">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G267" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
@@ -8220,14 +8216,14 @@
         <v>224</v>
       </c>
       <c r="D268" t="s">
-        <v>254</v>
+        <v>52</v>
       </c>
       <c r="E268" s="2"/>
       <c r="F268">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G268" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
@@ -8241,14 +8237,14 @@
         <v>224</v>
       </c>
       <c r="D269" t="s">
-        <v>110</v>
+        <v>254</v>
       </c>
       <c r="E269" s="2"/>
       <c r="F269">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G269" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -8262,14 +8258,14 @@
         <v>224</v>
       </c>
       <c r="D270" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E270" s="2"/>
       <c r="F270">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G270" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
@@ -8283,14 +8279,14 @@
         <v>224</v>
       </c>
       <c r="D271" t="s">
-        <v>266</v>
+        <v>121</v>
       </c>
       <c r="E271" s="2"/>
       <c r="F271">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G271" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
@@ -8300,18 +8296,18 @@
       <c r="B272" t="s">
         <v>205</v>
       </c>
-      <c r="C272" s="2" t="s">
+      <c r="C272" t="s">
         <v>224</v>
       </c>
-      <c r="D272" s="2" t="s">
-        <v>527</v>
+      <c r="D272" t="s">
+        <v>266</v>
       </c>
       <c r="E272" s="2"/>
-      <c r="F272" s="2">
-        <v>254</v>
-      </c>
-      <c r="G272" s="2" t="s">
-        <v>533</v>
+      <c r="F272">
+        <v>253</v>
+      </c>
+      <c r="G272" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
@@ -8321,18 +8317,18 @@
       <c r="B273" t="s">
         <v>205</v>
       </c>
-      <c r="C273" t="s">
-        <v>204</v>
-      </c>
-      <c r="D273" t="s">
-        <v>4</v>
+      <c r="C273" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D273" s="2" t="s">
+        <v>527</v>
       </c>
       <c r="E273" s="2"/>
-      <c r="F273">
-        <v>255</v>
-      </c>
-      <c r="G273" t="s">
-        <v>312</v>
+      <c r="F273" s="2">
+        <v>254</v>
+      </c>
+      <c r="G273" s="2" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
@@ -8346,14 +8342,14 @@
         <v>204</v>
       </c>
       <c r="D274" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E274" s="2"/>
       <c r="F274">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G274" t="s">
-        <v>454</v>
+        <v>312</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
@@ -8367,14 +8363,14 @@
         <v>204</v>
       </c>
       <c r="D275" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E275" s="2"/>
       <c r="F275">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G275" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
@@ -8388,14 +8384,14 @@
         <v>204</v>
       </c>
       <c r="D276" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
       <c r="E276" s="2"/>
       <c r="F276">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G276" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
@@ -8409,14 +8405,14 @@
         <v>204</v>
       </c>
       <c r="D277" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="E277" s="2"/>
       <c r="F277">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G277" t="s">
-        <v>334</v>
+        <v>455</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
@@ -8427,16 +8423,37 @@
         <v>205</v>
       </c>
       <c r="C278" t="s">
-        <v>264</v>
+        <v>204</v>
       </c>
       <c r="D278" t="s">
-        <v>264</v>
+        <v>169</v>
       </c>
       <c r="E278" s="2"/>
       <c r="F278">
+        <v>259</v>
+      </c>
+      <c r="G278" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>200</v>
+      </c>
+      <c r="B279" t="s">
+        <v>205</v>
+      </c>
+      <c r="C279" t="s">
+        <v>264</v>
+      </c>
+      <c r="D279" t="s">
+        <v>264</v>
+      </c>
+      <c r="E279" s="2"/>
+      <c r="F279">
         <v>260</v>
       </c>
-      <c r="G278" t="s">
+      <c r="G279" t="s">
         <v>492</v>
       </c>
     </row>

</xml_diff>